<commit_message>
Added additional options to heatmap and volcano options
</commit_message>
<xml_diff>
--- a/examples/TMT_Protein_List_Input_Example/data/raw/Fake_Example_TMT_Protein_List_Data.xlsx
+++ b/examples/TMT_Protein_List_Input_Example/data/raw/Fake_Example_TMT_Protein_List_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pelowitz.thomas/Documents/Analysis_Pipeline_Textual/examples/TMT_Protein_List_Input_Example/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5586152A-1A76-A045-BD96-61E736C1CEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB9E9DE-C1F5-2F4A-A167-BD6F277755B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="660" windowWidth="18960" windowHeight="21680" xr2:uid="{B9E7093A-6B5C-F24D-85AD-591186F340AC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{B9E7093A-6B5C-F24D-85AD-591186F340AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1679,16 +1679,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3962204B-783F-9A4A-9099-C2BF20394D85}">
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="105.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="250.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
     <col min="5" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="21" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -8210,8 +8210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3813E9E-541D-ED40-B847-463A5A6F902D}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8359,7 +8359,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8417,7 +8417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214411B5-98B2-5643-B649-6F8BDD7A57B1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>